<commit_message>
fixing the use of "/"
</commit_message>
<xml_diff>
--- a/AIS/SPARC4_Spectral_Response/analyser_extra_ordinary.xlsx
+++ b/AIS/SPARC4_Spectral_Response/analyser_extra_ordinary.xlsx
@@ -20,9 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="2">
   <si>
     <t xml:space="preserve">Analyser Extra Ordinary</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.5</t>
   </si>
 </sst>
 </file>
@@ -147,10 +150,10 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.68359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.83"/>
   </cols>
@@ -164,7 +167,7 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
@@ -181,7 +184,7 @@
       <c r="A3" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="n">
@@ -198,7 +201,7 @@
       <c r="B4" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="2" t="n">
@@ -215,7 +218,7 @@
       <c r="C5" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>